<commit_message>
Text editor format files, and some updates to classes
</commit_message>
<xml_diff>
--- a/src/test/resources/rewards_platform/test_data/LMS File Record Layouts.xlsx
+++ b/src/test/resources/rewards_platform/test_data/LMS File Record Layouts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariatkacheva/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariatkacheva/Documents/workspace/rewards_platform/src/test/resources/rewards_platform/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="460" windowWidth="11380" windowHeight="5060" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="-37760" yWindow="-1100" windowWidth="28800" windowHeight="16240" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="QPQP" sheetId="1" r:id="rId1"/>
@@ -84,11 +84,11 @@
     <definedName name="Z_DA9EBB5A_EE92_41AE_B134_012594BFFC70_.wvu.FilterData" localSheetId="1" hidden="1">QPQB!$C$6:$I$131</definedName>
     <definedName name="Z_DA9EBB5A_EE92_41AE_B134_012594BFFC70_.wvu.FilterData" localSheetId="0" hidden="1">QPQP!$B$5:$H$184</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="bjutta - Personal View" guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="794" activeSheetId="6"/>
+    <customWorkbookView name="gpadhiar - Personal View" guid="{99249448-FD30-4600-8F88-D8162E1600C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="794" activeSheetId="7"/>
     <customWorkbookView name="jdutta - Personal View" guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="794" activeSheetId="1"/>
-    <customWorkbookView name="gpadhiar - Personal View" guid="{99249448-FD30-4600-8F88-D8162E1600C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="794" activeSheetId="7"/>
-    <customWorkbookView name="bjutta - Personal View" guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="794" activeSheetId="6"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -13976,9 +13976,9 @@
   </sheetData>
   <autoFilter ref="B5:H184"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" showAutoFilter="1">
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H183" sqref="H183"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter>
@@ -13996,9 +13996,9 @@
       </headerFooter>
       <autoFilter ref="B1:H1"/>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" showAutoFilter="1">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H183" sqref="H183"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
       <headerFooter>
@@ -15211,13 +15211,14 @@
   </sheetData>
   <autoFilter ref="B5:H35"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A13">
-      <selection activeCell="I28" sqref="I28"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+      <selection activeCell="B5" sqref="B5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
+      <autoFilter ref="B1:H1"/>
     </customSheetView>
     <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}" topLeftCell="A10">
       <selection activeCell="C26" sqref="C26"/>
@@ -15227,14 +15228,13 @@
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
-      <selection activeCell="B5" sqref="B5"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A13">
+      <selection activeCell="I28" sqref="I28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
-      <autoFilter ref="B1:H1"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -22527,7 +22527,7 @@
   <dimension ref="A1:J2333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36662,8 +36662,8 @@
   </sheetData>
   <autoFilter ref="C6:I131"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" showAutoFilter="1" topLeftCell="A7">
-      <selection activeCell="I19" sqref="I19:I20"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+      <selection activeCell="I11" sqref="I11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
       <headerFooter>
@@ -36680,8 +36680,8 @@
       </headerFooter>
       <autoFilter ref="B1:H1"/>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
-      <selection activeCell="I11" sqref="I11"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" showAutoFilter="1" topLeftCell="A7">
+      <selection activeCell="I19" sqref="I19:I20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId3"/>
       <headerFooter>
@@ -61091,11 +61091,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B51:H51"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -61104,6 +61099,11 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B51:H51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -61465,8 +61465,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A7">
-      <selection activeCell="H14" sqref="H14"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
+      <selection activeCell="B2" sqref="B2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
       <headerFooter>
@@ -61482,8 +61482,8 @@
       </headerFooter>
       <autoFilter ref="B1:H1"/>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
-      <selection activeCell="B2" sqref="B2"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A7">
+      <selection activeCell="H14" sqref="H14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
       <headerFooter>
@@ -62060,8 +62060,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A11">
-      <selection activeCell="H26" sqref="H26"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
+      <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
       <headerFooter>
@@ -62077,8 +62077,8 @@
       </headerFooter>
       <autoFilter ref="B1:H1"/>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
-      <selection activeCell="B1" sqref="B1"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A11">
+      <selection activeCell="H26" sqref="H26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
       <headerFooter>
@@ -62622,8 +62622,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A4">
-      <selection activeCell="H9" sqref="H9"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
+      <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
       <headerFooter>
@@ -62639,8 +62639,8 @@
       </headerFooter>
       <autoFilter ref="B1:H1"/>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}">
-      <selection activeCell="B1" sqref="B1"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A4">
+      <selection activeCell="H9" sqref="H9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId3"/>
       <headerFooter>
@@ -63462,13 +63462,14 @@
   </sheetData>
   <autoFilter ref="B5:H42"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A10">
-      <selection activeCell="H37" sqref="H37"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
+      <autoFilter ref="B1:H1"/>
     </customSheetView>
     <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}" topLeftCell="A19">
       <selection activeCell="C51" sqref="C51"/>
@@ -63478,14 +63479,13 @@
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
-      <selection activeCell="B6" sqref="B6"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A10">
+      <selection activeCell="H37" sqref="H37"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
-      <autoFilter ref="B1:H1"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -64101,13 +64101,14 @@
   </sheetData>
   <autoFilter ref="B5:I29"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A16">
-      <selection activeCell="E34" sqref="E34"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
+      <autoFilter ref="B1:I1"/>
     </customSheetView>
     <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}" topLeftCell="A19">
       <selection activeCell="I29" sqref="I29"/>
@@ -64117,14 +64118,13 @@
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
-      <selection activeCell="B6" sqref="B6"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A16">
+      <selection activeCell="E34" sqref="E34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
-      <autoFilter ref="B1:I1"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -65518,26 +65518,10 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A58">
-      <selection activeCell="I11" sqref="I11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <headerFooter>
-        <oddFooter>&amp;LCapital One Confidential</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}" topLeftCell="A49">
-      <selection activeCell="E31" sqref="E31"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <headerFooter>
-        <oddFooter>&amp;LCapital One Confidential</oddFooter>
-      </headerFooter>
-    </customSheetView>
     <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" filter="1" showAutoFilter="1">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
@@ -65555,6 +65539,22 @@
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}" topLeftCell="A49">
+      <selection activeCell="E31" sqref="E31"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <headerFooter>
+        <oddFooter>&amp;LCapital One Confidential</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A58">
+      <selection activeCell="I11" sqref="I11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
+      <headerFooter>
+        <oddFooter>&amp;LCapital One Confidential</oddFooter>
+      </headerFooter>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -66071,13 +66071,14 @@
   </sheetData>
   <autoFilter ref="B5:H27"/>
   <customSheetViews>
-    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A7">
-      <selection activeCell="I19" sqref="I19"/>
+    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
+      <autoFilter ref="B1:H1"/>
     </customSheetView>
     <customSheetView guid="{99249448-FD30-4600-8F88-D8162E1600C3}">
       <selection activeCell="I19" sqref="I19"/>
@@ -66087,14 +66088,13 @@
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A9143449-51F8-4013-8046-64C4C1DF5386}" showAutoFilter="1">
-      <selection activeCell="B6" sqref="B6"/>
+    <customSheetView guid="{6CF6AD5B-3115-4DC4-8567-E2497412C005}" topLeftCell="A7">
+      <selection activeCell="I19" sqref="I19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId3"/>
       <headerFooter>
         <oddFooter>&amp;LCapital One Confidential</oddFooter>
       </headerFooter>
-      <autoFilter ref="B1:H1"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>